<commit_message>
Finished testing and added gitignore
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0D05D-5AF7-46F5-9BA2-DD0C1874C8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195075F7-CE7E-4BB6-8B07-CF3B3851A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>

</xml_diff>

<commit_message>
Visualisation of diffusion nodes
Made a visualisation of the bacteria, the grid centres, the initial diffusion nodes and the final diffusion nodes. This includes the boundary layer circle of bacteria as a check.
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195075F7-CE7E-4BB6-8B07-CF3B3851A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A7B403-6356-4A61-AA2E-E04CE5691030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -1408,7 +1408,7 @@
     <t>Add columns with per bacterial species the Ks values [M] per substrate. Make sure that the compound and bacterium names match the rest of the Excel file</t>
   </si>
   <si>
-    <t>suspension</t>
+    <t>granule</t>
   </si>
 </sst>
 </file>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="B3" s="248" t="str">
         <f>Bacteria!B6</f>
-        <v>suspension</v>
+        <v>granule</v>
       </c>
       <c r="C3" s="262"/>
     </row>
@@ -9564,7 +9564,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adjusted plot blayer nodes file
Saved plots and adjusted bacterial size
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A7B403-6356-4A61-AA2E-E04CE5691030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62F188-EB4C-4BF0-9A36-3AB2A7DA8F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9564,7 +9564,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added tests for general lib files
Wrote tests and moved the struct definition to an file where it is its own module
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62F188-EB4C-4BF0-9A36-3AB2A7DA8F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C24E6FC-0BAC-47A7-BABD-2CD8D26EF6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -8462,7 +8462,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8536,7 +8536,7 @@
       </c>
       <c r="B6" s="248" t="b">
         <f>Solver!B4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="262"/>
     </row>
@@ -8547,7 +8547,7 @@
       </c>
       <c r="B7" s="248" t="b">
         <f>Solver!B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="262"/>
     </row>
@@ -8558,7 +8558,7 @@
       </c>
       <c r="B8" s="249" t="b">
         <f>Solver!B5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="262"/>
     </row>
@@ -8569,7 +8569,7 @@
       </c>
       <c r="B9" s="248" t="b">
         <f>Solver!B11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="262"/>
     </row>
@@ -9563,7 +9563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -9864,8 +9864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9893,7 +9893,7 @@
         <v>201</v>
       </c>
       <c r="B2" s="122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>90</v>
@@ -9921,7 +9921,7 @@
         <v>230</v>
       </c>
       <c r="B4" s="122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>90</v>
@@ -9935,7 +9935,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>90</v>
@@ -10019,7 +10019,7 @@
         <v>233</v>
       </c>
       <c r="B11" s="122" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="90" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Implemented general Detachment functions
Implemented calcTimeOfDetach and calculateLocalDetachmentRate.
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C24E6FC-0BAC-47A7-BABD-2CD8D26EF6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C888970-EA04-4977-86C6-6D41F00A0868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -9563,8 +9563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9864,7 +9864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>